<commit_message>
Bulk Upload Final changes
</commit_message>
<xml_diff>
--- a/src/test/resources/Files/Exam Takers Template.xlsx
+++ b/src/test/resources/Files/Exam Takers Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="366">
   <si>
     <t>FirstName</t>
   </si>
@@ -752,6 +752,366 @@
   </si>
   <si>
     <t>95826</t>
+  </si>
+  <si>
+    <t>Examtaker67234</t>
+  </si>
+  <si>
+    <t>Automation67234</t>
+  </si>
+  <si>
+    <t>examtakerautomation67234@gmail.com</t>
+  </si>
+  <si>
+    <t>67234</t>
+  </si>
+  <si>
+    <t>Examtaker67780</t>
+  </si>
+  <si>
+    <t>Automation67780</t>
+  </si>
+  <si>
+    <t>examtakerautomation67780@gmail.com</t>
+  </si>
+  <si>
+    <t>67780</t>
+  </si>
+  <si>
+    <t>Examtaker99976</t>
+  </si>
+  <si>
+    <t>Automation99976</t>
+  </si>
+  <si>
+    <t>examtakerautomation99976@gmail.com</t>
+  </si>
+  <si>
+    <t>99976</t>
+  </si>
+  <si>
+    <t>Examtaker96782</t>
+  </si>
+  <si>
+    <t>Automation96782</t>
+  </si>
+  <si>
+    <t>examtakerautomation96782@gmail.com</t>
+  </si>
+  <si>
+    <t>96782</t>
+  </si>
+  <si>
+    <t>Examtaker23971</t>
+  </si>
+  <si>
+    <t>Automation23971</t>
+  </si>
+  <si>
+    <t>examtakerautomation23971@gmail.com</t>
+  </si>
+  <si>
+    <t>23971</t>
+  </si>
+  <si>
+    <t>Examtaker44871</t>
+  </si>
+  <si>
+    <t>Automation44871</t>
+  </si>
+  <si>
+    <t>examtakerautomation44871@gmail.com</t>
+  </si>
+  <si>
+    <t>44871</t>
+  </si>
+  <si>
+    <t>Examtaker91744</t>
+  </si>
+  <si>
+    <t>Automation91744</t>
+  </si>
+  <si>
+    <t>examtakerautomation91744@gmail.com</t>
+  </si>
+  <si>
+    <t>91744</t>
+  </si>
+  <si>
+    <t>Examtaker83268</t>
+  </si>
+  <si>
+    <t>Automation83268</t>
+  </si>
+  <si>
+    <t>examtakerautomation83268@gmail.com</t>
+  </si>
+  <si>
+    <t>83268</t>
+  </si>
+  <si>
+    <t>Examtaker19536</t>
+  </si>
+  <si>
+    <t>Automation19536</t>
+  </si>
+  <si>
+    <t>examtakerautomation19536@gmail.com</t>
+  </si>
+  <si>
+    <t>19536</t>
+  </si>
+  <si>
+    <t>Examtaker45715</t>
+  </si>
+  <si>
+    <t>Automation45715</t>
+  </si>
+  <si>
+    <t>examtakerautomation45715@gmail.com</t>
+  </si>
+  <si>
+    <t>45715</t>
+  </si>
+  <si>
+    <t>Examtaker01631</t>
+  </si>
+  <si>
+    <t>Automation01631</t>
+  </si>
+  <si>
+    <t>examtakerautomation01631@gmail.com</t>
+  </si>
+  <si>
+    <t>01631</t>
+  </si>
+  <si>
+    <t>Examtaker91177</t>
+  </si>
+  <si>
+    <t>Automation91177</t>
+  </si>
+  <si>
+    <t>examtakerautomation91177@gmail.com</t>
+  </si>
+  <si>
+    <t>91177</t>
+  </si>
+  <si>
+    <t>Examtaker19514</t>
+  </si>
+  <si>
+    <t>Automation19514</t>
+  </si>
+  <si>
+    <t>examtakerautomation19514@gmail.com</t>
+  </si>
+  <si>
+    <t>19514</t>
+  </si>
+  <si>
+    <t>Examtaker25968</t>
+  </si>
+  <si>
+    <t>Automation25968</t>
+  </si>
+  <si>
+    <t>examtakerautomation25968@gmail.com</t>
+  </si>
+  <si>
+    <t>25968</t>
+  </si>
+  <si>
+    <t>Examtaker66463</t>
+  </si>
+  <si>
+    <t>Automation66463</t>
+  </si>
+  <si>
+    <t>examtakerautomation66463@gmail.com</t>
+  </si>
+  <si>
+    <t>66463</t>
+  </si>
+  <si>
+    <t>Examtaker49863</t>
+  </si>
+  <si>
+    <t>Automation49863</t>
+  </si>
+  <si>
+    <t>examtakerautomation49863@gmail.com</t>
+  </si>
+  <si>
+    <t>49863</t>
+  </si>
+  <si>
+    <t>Examtaker62120</t>
+  </si>
+  <si>
+    <t>Automation62120</t>
+  </si>
+  <si>
+    <t>examtakerautomation62120@gmail.com</t>
+  </si>
+  <si>
+    <t>62120</t>
+  </si>
+  <si>
+    <t>Examtaker89069</t>
+  </si>
+  <si>
+    <t>Automation89069</t>
+  </si>
+  <si>
+    <t>examtakerautomation89069@gmail.com</t>
+  </si>
+  <si>
+    <t>89069</t>
+  </si>
+  <si>
+    <t>Examtaker24311</t>
+  </si>
+  <si>
+    <t>Automation24311</t>
+  </si>
+  <si>
+    <t>examtakerautomation24311@gmail.com</t>
+  </si>
+  <si>
+    <t>24311</t>
+  </si>
+  <si>
+    <t>Examtaker57572</t>
+  </si>
+  <si>
+    <t>Automation57572</t>
+  </si>
+  <si>
+    <t>examtakerautomation57572@gmail.com</t>
+  </si>
+  <si>
+    <t>57572</t>
+  </si>
+  <si>
+    <t>Examtaker47847</t>
+  </si>
+  <si>
+    <t>Automation47847</t>
+  </si>
+  <si>
+    <t>examtakerautomation47847@gmail.com</t>
+  </si>
+  <si>
+    <t>47847</t>
+  </si>
+  <si>
+    <t>Examtaker38505</t>
+  </si>
+  <si>
+    <t>Automation38505</t>
+  </si>
+  <si>
+    <t>examtakerautomation38505@gmail.com</t>
+  </si>
+  <si>
+    <t>38505</t>
+  </si>
+  <si>
+    <t>Examtaker27293</t>
+  </si>
+  <si>
+    <t>Automation27293</t>
+  </si>
+  <si>
+    <t>examtakerautomation27293@gmail.com</t>
+  </si>
+  <si>
+    <t>27293</t>
+  </si>
+  <si>
+    <t>Examtaker59284</t>
+  </si>
+  <si>
+    <t>Automation59284</t>
+  </si>
+  <si>
+    <t>examtakerautomation59284@gmail.com</t>
+  </si>
+  <si>
+    <t>59284</t>
+  </si>
+  <si>
+    <t>Examtaker12605</t>
+  </si>
+  <si>
+    <t>Automation12605</t>
+  </si>
+  <si>
+    <t>examtakerautomation12605@gmail.com</t>
+  </si>
+  <si>
+    <t>12605</t>
+  </si>
+  <si>
+    <t>Examtaker43609</t>
+  </si>
+  <si>
+    <t>Automation43609</t>
+  </si>
+  <si>
+    <t>examtakerautomation43609@gmail.com</t>
+  </si>
+  <si>
+    <t>43609</t>
+  </si>
+  <si>
+    <t>Examtaker30736</t>
+  </si>
+  <si>
+    <t>Automation30736</t>
+  </si>
+  <si>
+    <t>examtakerautomation30736@gmail.com</t>
+  </si>
+  <si>
+    <t>30736</t>
+  </si>
+  <si>
+    <t>Examtaker71699</t>
+  </si>
+  <si>
+    <t>Automation71699</t>
+  </si>
+  <si>
+    <t>examtakerautomation71699@gmail.com</t>
+  </si>
+  <si>
+    <t>71699</t>
+  </si>
+  <si>
+    <t>Examtaker20065</t>
+  </si>
+  <si>
+    <t>Automation20065</t>
+  </si>
+  <si>
+    <t>examtakerautomation20065@gmail.com</t>
+  </si>
+  <si>
+    <t>20065</t>
+  </si>
+  <si>
+    <t>Examtaker28138</t>
+  </si>
+  <si>
+    <t>Automation28138</t>
+  </si>
+  <si>
+    <t>examtakerautomation28138@gmail.com</t>
+  </si>
+  <si>
+    <t>28138</t>
   </si>
 </sst>
 </file>
@@ -1162,422 +1522,422 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>247</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>251</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>252</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>254</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>255</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>256</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>258</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>259</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>260</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>262</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>263</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>264</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>266</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>267</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>268</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>270</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>271</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>272</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>274</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>275</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>276</v>
       </c>
       <c r="D9" t="s">
-        <v>157</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>278</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>279</v>
       </c>
       <c r="C10" t="s">
-        <v>160</v>
+        <v>280</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>282</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>283</v>
       </c>
       <c r="C11" t="s">
-        <v>164</v>
+        <v>284</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>286</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>287</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>288</v>
       </c>
       <c r="D12" t="s">
-        <v>169</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>290</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>291</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>292</v>
       </c>
       <c r="D13" t="s">
-        <v>173</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>294</v>
       </c>
       <c r="B14" t="s">
-        <v>175</v>
+        <v>295</v>
       </c>
       <c r="C14" t="s">
-        <v>176</v>
+        <v>296</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>298</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
+        <v>299</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="D15" t="s">
-        <v>181</v>
+        <v>301</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>302</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>303</v>
       </c>
       <c r="C16" t="s">
-        <v>184</v>
+        <v>304</v>
       </c>
       <c r="D16" t="s">
-        <v>185</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>186</v>
+        <v>306</v>
       </c>
       <c r="B17" t="s">
-        <v>187</v>
+        <v>307</v>
       </c>
       <c r="C17" t="s">
-        <v>188</v>
+        <v>308</v>
       </c>
       <c r="D17" t="s">
-        <v>189</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>190</v>
+        <v>310</v>
       </c>
       <c r="B18" t="s">
-        <v>191</v>
+        <v>311</v>
       </c>
       <c r="C18" t="s">
-        <v>192</v>
+        <v>312</v>
       </c>
       <c r="D18" t="s">
-        <v>193</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>314</v>
       </c>
       <c r="B19" t="s">
-        <v>195</v>
+        <v>315</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>316</v>
       </c>
       <c r="D19" t="s">
-        <v>197</v>
+        <v>317</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>198</v>
+        <v>318</v>
       </c>
       <c r="B20" t="s">
-        <v>199</v>
+        <v>319</v>
       </c>
       <c r="C20" t="s">
-        <v>200</v>
+        <v>320</v>
       </c>
       <c r="D20" t="s">
-        <v>201</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>202</v>
+        <v>322</v>
       </c>
       <c r="B21" t="s">
-        <v>203</v>
+        <v>323</v>
       </c>
       <c r="C21" t="s">
-        <v>204</v>
+        <v>324</v>
       </c>
       <c r="D21" t="s">
-        <v>205</v>
+        <v>325</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>206</v>
+        <v>326</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>327</v>
       </c>
       <c r="C22" t="s">
-        <v>208</v>
+        <v>328</v>
       </c>
       <c r="D22" t="s">
-        <v>209</v>
+        <v>329</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>210</v>
+        <v>330</v>
       </c>
       <c r="B23" t="s">
-        <v>211</v>
+        <v>331</v>
       </c>
       <c r="C23" t="s">
-        <v>212</v>
+        <v>332</v>
       </c>
       <c r="D23" t="s">
-        <v>213</v>
+        <v>333</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>214</v>
+        <v>334</v>
       </c>
       <c r="B24" t="s">
-        <v>215</v>
+        <v>335</v>
       </c>
       <c r="C24" t="s">
-        <v>216</v>
+        <v>336</v>
       </c>
       <c r="D24" t="s">
-        <v>217</v>
+        <v>337</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>218</v>
+        <v>338</v>
       </c>
       <c r="B25" t="s">
-        <v>219</v>
+        <v>339</v>
       </c>
       <c r="C25" t="s">
-        <v>220</v>
+        <v>340</v>
       </c>
       <c r="D25" t="s">
-        <v>221</v>
+        <v>341</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>222</v>
+        <v>342</v>
       </c>
       <c r="B26" t="s">
-        <v>223</v>
+        <v>343</v>
       </c>
       <c r="C26" t="s">
-        <v>224</v>
+        <v>344</v>
       </c>
       <c r="D26" t="s">
-        <v>225</v>
+        <v>345</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>226</v>
+        <v>346</v>
       </c>
       <c r="B27" t="s">
-        <v>227</v>
+        <v>347</v>
       </c>
       <c r="C27" t="s">
-        <v>228</v>
+        <v>348</v>
       </c>
       <c r="D27" t="s">
-        <v>229</v>
+        <v>349</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>230</v>
+        <v>350</v>
       </c>
       <c r="B28" t="s">
-        <v>231</v>
+        <v>351</v>
       </c>
       <c r="C28" t="s">
-        <v>232</v>
+        <v>352</v>
       </c>
       <c r="D28" t="s">
-        <v>233</v>
+        <v>353</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>234</v>
+        <v>354</v>
       </c>
       <c r="B29" t="s">
-        <v>235</v>
+        <v>355</v>
       </c>
       <c r="C29" t="s">
-        <v>236</v>
+        <v>356</v>
       </c>
       <c r="D29" t="s">
-        <v>237</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>238</v>
+        <v>358</v>
       </c>
       <c r="B30" t="s">
-        <v>239</v>
+        <v>359</v>
       </c>
       <c r="C30" t="s">
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="D30" t="s">
-        <v>241</v>
+        <v>361</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>242</v>
+        <v>362</v>
       </c>
       <c r="B31" t="s">
-        <v>243</v>
+        <v>363</v>
       </c>
       <c r="C31" t="s">
-        <v>244</v>
+        <v>364</v>
       </c>
       <c r="D31" t="s">
-        <v>245</v>
+        <v>365</v>
       </c>
     </row>
     <row r="32"/>

</xml_diff>